<commit_message>
BI report view and measure tracking\Commercial BI-NTDL Report List Updated
</commit_message>
<xml_diff>
--- a/BI report view and measure tracking.xlsx
+++ b/BI report view and measure tracking.xlsx
@@ -8,19 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA740DD-959F-44A2-8F9A-3DA69125D424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54039E42-0D01-471D-BEBD-8200996CCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" activeTab="1" xr2:uid="{F003A2DB-3BC2-407F-B939-8F4975B88621}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{F003A2DB-3BC2-407F-B939-8F4975B88621}"/>
   </bookViews>
   <sheets>
-    <sheet name="Native Dashboard" sheetId="6" r:id="rId1"/>
-    <sheet name="BI Report for NTDL (All)" sheetId="2" r:id="rId2"/>
-    <sheet name="BI Report for NTDL" sheetId="3" r:id="rId3"/>
-    <sheet name="BI Report for NTTML" sheetId="1" r:id="rId4"/>
-    <sheet name="Employee Attendance Status" sheetId="4" r:id="rId5"/>
-    <sheet name="Production Reconciliation" sheetId="5" r:id="rId6"/>
+    <sheet name="Commercial BI-NTDL" sheetId="7" r:id="rId1"/>
+    <sheet name="Native Dashboard" sheetId="6" r:id="rId2"/>
+    <sheet name="BI Report for NTDL (All)" sheetId="2" r:id="rId3"/>
+    <sheet name="BI Report for NTDL" sheetId="3" r:id="rId4"/>
+    <sheet name="BI Report for NTTML" sheetId="1" r:id="rId5"/>
+    <sheet name="Employee Attendance Status" sheetId="4" r:id="rId6"/>
+    <sheet name="Production Reconciliation" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Commercial BI-NTDL'!$A$1:$B$1</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="361">
   <si>
     <t>Fabric Stock Ageing</t>
   </si>
@@ -1105,6 +1109,18 @@
   </si>
   <si>
     <t>M/ Outside W/out Per Now</t>
+  </si>
+  <si>
+    <t>Export LC Register (PI Based)</t>
+  </si>
+  <si>
+    <t>Export Document Submission Statement</t>
+  </si>
+  <si>
+    <t>Export Document Realization Statement</t>
+  </si>
+  <si>
+    <t>LC Receiving Status</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1384,6 +1400,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1697,6 +1714,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CEA0AA-87B7-4214-9520-C48ADED93576}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{F8CEA0AA-87B7-4214-9520-C48ADED93576}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE189463-EA32-4A14-B5C4-9BDA85241456}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1833,13 +1974,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF53609E-9AE9-4EB6-8F3A-B5042303457D}">
   <dimension ref="A1:L235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16:C21"/>
+      <selection pane="topRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3938,12 +4079,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="C50:C65"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="C33:C46"/>
     <mergeCell ref="C98:C102"/>
     <mergeCell ref="C91:C94"/>
     <mergeCell ref="C185:C208"/>
@@ -3955,18 +4090,24 @@
     <mergeCell ref="C129:C133"/>
     <mergeCell ref="C117:C125"/>
     <mergeCell ref="C106:C113"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="C50:C65"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="C33:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5131CFE0-5081-42CE-BE72-FFCC175BE355}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4076,13 +4217,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258D56AF-3DBD-4AAA-8F11-8DBE6CBF5F22}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G36" sqref="G36:G40"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4594,7 +4735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FA286F-2DA1-404F-9D6A-C9EFFCEE0390}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -4850,7 +4991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1190D3CE-578C-487D-8A5C-7F9D5ABD35C0}">
   <dimension ref="A1:H32"/>
   <sheetViews>

</xml_diff>

<commit_message>
Commercial BI\Pending Acceptance Statement (Export)
</commit_message>
<xml_diff>
--- a/BI report view and measure tracking.xlsx
+++ b/BI report view and measure tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54039E42-0D01-471D-BEBD-8200996CCDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC4C1C2-0922-419B-9E37-8DD35342DD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{F003A2DB-3BC2-407F-B939-8F4975B88621}"/>
   </bookViews>
@@ -1160,7 +1160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1182,6 +1182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1307,7 +1313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1376,6 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1400,7 +1407,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1715,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CEA0AA-87B7-4214-9520-C48ADED93576}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,10 +1737,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="26" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1743,90 +1753,99 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="A6" s="35">
+        <v>6</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
+      <c r="A7" s="35">
+        <v>7</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>357</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>358</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>360</v>
       </c>
     </row>
@@ -1855,13 +1874,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1881,7 +1900,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1898,7 +1917,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
@@ -1911,7 +1930,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1920,7 +1939,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1929,7 +1948,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1938,7 +1957,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1947,7 +1966,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1956,7 +1975,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2028,7 +2047,7 @@
       <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2045,7 +2064,7 @@
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="8" t="s">
         <v>56</v>
       </c>
@@ -2058,7 +2077,7 @@
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="8" t="s">
         <v>57</v>
       </c>
@@ -2071,7 +2090,7 @@
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="8" t="s">
         <v>58</v>
       </c>
@@ -2084,7 +2103,7 @@
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="8" t="s">
         <v>59</v>
       </c>
@@ -2097,7 +2116,7 @@
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="8" t="s">
         <v>60</v>
       </c>
@@ -2110,7 +2129,7 @@
       <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="27"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="8" t="s">
         <v>61</v>
       </c>
@@ -2119,7 +2138,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="C10" s="27"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="8" t="s">
         <v>69</v>
       </c>
@@ -2128,7 +2147,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="C11" s="27"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="8" t="s">
         <v>71</v>
       </c>
@@ -2139,7 +2158,7 @@
       <c r="A12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="8" t="s">
         <v>70</v>
       </c>
@@ -2206,7 +2225,7 @@
       <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -2241,7 +2260,7 @@
       <c r="A17" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="29"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -2264,7 +2283,7 @@
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -2287,7 +2306,7 @@
       <c r="A19" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -2307,7 +2326,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="29"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -2330,7 +2349,7 @@
       <c r="A21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -2382,7 +2401,7 @@
       <c r="A25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -2397,7 +2416,7 @@
       <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="29"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="8" t="s">
         <v>109</v>
       </c>
@@ -2408,7 +2427,7 @@
       <c r="A27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="29"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="8" t="s">
         <v>110</v>
       </c>
@@ -2419,7 +2438,7 @@
       <c r="A28" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="29"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="8" t="s">
         <v>111</v>
       </c>
@@ -2427,7 +2446,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="30"/>
+      <c r="C29" s="31"/>
       <c r="D29" s="8" t="s">
         <v>115</v>
       </c>
@@ -2452,7 +2471,7 @@
       <c r="F32" s="10"/>
     </row>
     <row r="33" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -2462,7 +2481,7 @@
       <c r="F33" s="10"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="26"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="8" t="s">
         <v>118</v>
       </c>
@@ -2470,7 +2489,7 @@
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="26"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="8" t="s">
         <v>119</v>
       </c>
@@ -2478,7 +2497,7 @@
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="26"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="8" t="s">
         <v>120</v>
       </c>
@@ -2486,7 +2505,7 @@
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="8" t="s">
         <v>121</v>
       </c>
@@ -2494,7 +2513,7 @@
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="26"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="8" t="s">
         <v>128</v>
       </c>
@@ -2502,7 +2521,7 @@
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="26"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="8" t="s">
         <v>122</v>
       </c>
@@ -2510,7 +2529,7 @@
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="26"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="8" t="s">
         <v>123</v>
       </c>
@@ -2518,7 +2537,7 @@
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="26"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="8" t="s">
         <v>124</v>
       </c>
@@ -2526,7 +2545,7 @@
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="26"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="8" t="s">
         <v>125</v>
       </c>
@@ -2534,25 +2553,25 @@
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="26"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="26"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="26"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="26"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="8" t="s">
         <v>127</v>
       </c>
@@ -2575,7 +2594,7 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D50" s="7" t="s">
@@ -2585,7 +2604,7 @@
       <c r="F50" s="10"/>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="26"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="8" t="s">
         <v>132</v>
       </c>
@@ -2593,7 +2612,7 @@
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="26"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="8" t="s">
         <v>133</v>
       </c>
@@ -2601,7 +2620,7 @@
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="26"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="8" t="s">
         <v>134</v>
       </c>
@@ -2609,7 +2628,7 @@
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="26"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="8" t="s">
         <v>137</v>
       </c>
@@ -2617,7 +2636,7 @@
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="26"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="8" t="s">
         <v>135</v>
       </c>
@@ -2625,7 +2644,7 @@
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="26"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="8" t="s">
         <v>136</v>
       </c>
@@ -2633,7 +2652,7 @@
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="26"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="8" t="s">
         <v>138</v>
       </c>
@@ -2641,7 +2660,7 @@
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="26"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="8" t="s">
         <v>139</v>
       </c>
@@ -2649,7 +2668,7 @@
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="26"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="8" t="s">
         <v>140</v>
       </c>
@@ -2657,37 +2676,37 @@
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="26"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="26"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="8" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="26"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="26"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="8" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="26"/>
+      <c r="C64" s="27"/>
       <c r="D64" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C65" s="26"/>
+      <c r="C65" s="27"/>
       <c r="D65" s="8" t="s">
         <v>145</v>
       </c>
@@ -2726,7 +2745,7 @@
       </c>
     </row>
     <row r="69" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="28" t="s">
+      <c r="C69" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D69" s="7" t="s">
@@ -2749,7 +2768,7 @@
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C70" s="29"/>
+      <c r="C70" s="30"/>
       <c r="D70" s="8" t="s">
         <v>149</v>
       </c>
@@ -2766,7 +2785,7 @@
       <c r="I70" s="8"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="29"/>
+      <c r="C71" s="30"/>
       <c r="D71" s="8" t="s">
         <v>160</v>
       </c>
@@ -2783,7 +2802,7 @@
       <c r="I71" s="8"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C72" s="29"/>
+      <c r="C72" s="30"/>
       <c r="D72" s="8" t="s">
         <v>161</v>
       </c>
@@ -2798,7 +2817,7 @@
       <c r="I72" s="8"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C73" s="29"/>
+      <c r="C73" s="30"/>
       <c r="D73" s="8" t="s">
         <v>163</v>
       </c>
@@ -2811,7 +2830,7 @@
       <c r="I73" s="8"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C74" s="30"/>
+      <c r="C74" s="31"/>
       <c r="D74" s="8" t="s">
         <v>164</v>
       </c>
@@ -2857,7 +2876,7 @@
       </c>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C78" s="26" t="s">
+      <c r="C78" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D78" s="7" t="s">
@@ -2877,7 +2896,7 @@
       </c>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C79" s="27"/>
+      <c r="C79" s="28"/>
       <c r="D79" s="8" t="s">
         <v>161</v>
       </c>
@@ -2891,7 +2910,7 @@
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="27"/>
+      <c r="C80" s="28"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8" t="s">
         <v>171</v>
@@ -2901,7 +2920,7 @@
       <c r="H80" s="8"/>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C81" s="27"/>
+      <c r="C81" s="28"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
         <v>119</v>
@@ -2911,7 +2930,7 @@
       <c r="H81" s="8"/>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C82" s="27"/>
+      <c r="C82" s="28"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8" t="s">
         <v>172</v>
@@ -2921,7 +2940,7 @@
       <c r="H82" s="8"/>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C83" s="27"/>
+      <c r="C83" s="28"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8" t="s">
         <v>125</v>
@@ -2931,7 +2950,7 @@
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="27"/>
+      <c r="C84" s="28"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8" t="s">
         <v>173</v>
@@ -2941,7 +2960,7 @@
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C85" s="27"/>
+      <c r="C85" s="28"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
         <v>174</v>
@@ -2951,7 +2970,7 @@
       <c r="H85" s="8"/>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C86" s="27"/>
+      <c r="C86" s="28"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
         <v>175</v>
@@ -2961,7 +2980,7 @@
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="27"/>
+      <c r="C87" s="28"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8" t="s">
         <v>176</v>
@@ -2991,7 +3010,7 @@
       </c>
     </row>
     <row r="91" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C91" s="28" t="s">
+      <c r="C91" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D91" s="7" t="s">
@@ -3005,7 +3024,7 @@
       </c>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C92" s="29"/>
+      <c r="C92" s="30"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8" t="s">
         <v>179</v>
@@ -3013,7 +3032,7 @@
       <c r="F92" s="8"/>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C93" s="29"/>
+      <c r="C93" s="30"/>
       <c r="D93" s="8"/>
       <c r="E93" s="8" t="s">
         <v>180</v>
@@ -3021,7 +3040,7 @@
       <c r="F93" s="8"/>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="30"/>
+      <c r="C94" s="31"/>
       <c r="D94" s="8"/>
       <c r="E94" s="8" t="s">
         <v>69</v>
@@ -3045,7 +3064,7 @@
       <c r="F97" s="10"/>
     </row>
     <row r="98" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C98" s="28" t="s">
+      <c r="C98" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D98" s="7" t="s">
@@ -3055,7 +3074,7 @@
       <c r="F98" s="10"/>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C99" s="29"/>
+      <c r="C99" s="30"/>
       <c r="D99" s="8" t="s">
         <v>186</v>
       </c>
@@ -3063,7 +3082,7 @@
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C100" s="29"/>
+      <c r="C100" s="30"/>
       <c r="D100" s="8" t="s">
         <v>187</v>
       </c>
@@ -3071,7 +3090,7 @@
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="29"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="8" t="s">
         <v>188</v>
       </c>
@@ -3079,7 +3098,7 @@
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C102" s="30"/>
+      <c r="C102" s="31"/>
       <c r="D102" s="8" t="s">
         <v>189</v>
       </c>
@@ -3103,7 +3122,7 @@
       </c>
     </row>
     <row r="106" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="28" t="s">
+      <c r="C106" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D106" s="7" t="s">
@@ -3114,49 +3133,49 @@
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C107" s="29"/>
+      <c r="C107" s="30"/>
       <c r="D107" s="8"/>
       <c r="E107" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="29"/>
+      <c r="C108" s="30"/>
       <c r="D108" s="8"/>
       <c r="E108" s="9" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C109" s="29"/>
+      <c r="C109" s="30"/>
       <c r="D109" s="8"/>
       <c r="E109" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C110" s="29"/>
+      <c r="C110" s="30"/>
       <c r="D110" s="8"/>
       <c r="E110" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C111" s="29"/>
+      <c r="C111" s="30"/>
       <c r="D111" s="8"/>
       <c r="E111" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C112" s="29"/>
+      <c r="C112" s="30"/>
       <c r="D112" s="8"/>
       <c r="E112" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C113" s="30"/>
+      <c r="C113" s="31"/>
       <c r="D113" s="8"/>
       <c r="E113" s="9" t="s">
         <v>187</v>
@@ -3179,7 +3198,7 @@
       </c>
     </row>
     <row r="117" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C117" s="28" t="s">
+      <c r="C117" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D117" s="7" t="s">
@@ -3190,56 +3209,56 @@
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C118" s="29"/>
+      <c r="C118" s="30"/>
       <c r="D118" s="8"/>
       <c r="E118" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C119" s="29"/>
+      <c r="C119" s="30"/>
       <c r="D119" s="8"/>
       <c r="E119" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="120" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C120" s="29"/>
+      <c r="C120" s="30"/>
       <c r="D120" s="8"/>
       <c r="E120" s="9" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C121" s="29"/>
+      <c r="C121" s="30"/>
       <c r="D121" s="8"/>
       <c r="E121" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="122" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C122" s="29"/>
+      <c r="C122" s="30"/>
       <c r="D122" s="8"/>
       <c r="E122" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="123" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C123" s="29"/>
+      <c r="C123" s="30"/>
       <c r="D123" s="8"/>
       <c r="E123" s="9" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C124" s="29"/>
+      <c r="C124" s="30"/>
       <c r="D124" s="8"/>
       <c r="E124" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C125" s="30"/>
+      <c r="C125" s="31"/>
       <c r="D125" s="8"/>
       <c r="E125" s="9" t="s">
         <v>189</v>
@@ -3262,7 +3281,7 @@
       </c>
     </row>
     <row r="129" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C129" s="28" t="s">
+      <c r="C129" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D129" s="7" t="s">
@@ -3273,28 +3292,28 @@
       </c>
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C130" s="29"/>
+      <c r="C130" s="30"/>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="29"/>
+      <c r="C131" s="30"/>
       <c r="D131" s="8"/>
       <c r="E131" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C132" s="29"/>
+      <c r="C132" s="30"/>
       <c r="D132" s="8"/>
       <c r="E132" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C133" s="30"/>
+      <c r="C133" s="31"/>
       <c r="D133" s="8"/>
       <c r="E133" s="9" t="s">
         <v>197</v>
@@ -3323,7 +3342,7 @@
       </c>
     </row>
     <row r="137" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C137" s="28" t="s">
+      <c r="C137" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D137" s="7" t="s">
@@ -3340,7 +3359,7 @@
       </c>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C138" s="29"/>
+      <c r="C138" s="30"/>
       <c r="D138" s="8" t="s">
         <v>77</v>
       </c>
@@ -3351,7 +3370,7 @@
       <c r="G138" s="9"/>
     </row>
     <row r="139" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C139" s="29"/>
+      <c r="C139" s="30"/>
       <c r="D139" s="8"/>
       <c r="E139" s="9"/>
       <c r="F139" s="9" t="s">
@@ -3360,7 +3379,7 @@
       <c r="G139" s="9"/>
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C140" s="29"/>
+      <c r="C140" s="30"/>
       <c r="D140" s="8"/>
       <c r="E140" s="9"/>
       <c r="F140" s="9" t="s">
@@ -3369,7 +3388,7 @@
       <c r="G140" s="9"/>
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C141" s="29"/>
+      <c r="C141" s="30"/>
       <c r="D141" s="8"/>
       <c r="E141" s="9"/>
       <c r="F141" s="9" t="s">
@@ -3378,7 +3397,7 @@
       <c r="G141" s="9"/>
     </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C142" s="29"/>
+      <c r="C142" s="30"/>
       <c r="D142" s="8"/>
       <c r="E142" s="9"/>
       <c r="F142" s="9" t="s">
@@ -3387,7 +3406,7 @@
       <c r="G142" s="9"/>
     </row>
     <row r="143" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C143" s="29"/>
+      <c r="C143" s="30"/>
       <c r="D143" s="8"/>
       <c r="E143" s="9"/>
       <c r="F143" s="9" t="s">
@@ -3396,7 +3415,7 @@
       <c r="G143" s="9"/>
     </row>
     <row r="144" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C144" s="30"/>
+      <c r="C144" s="31"/>
       <c r="D144" s="8"/>
       <c r="E144" s="9"/>
       <c r="F144" s="9" t="s">
@@ -3423,7 +3442,7 @@
       <c r="G147" s="10"/>
     </row>
     <row r="148" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C148" s="31" t="s">
+      <c r="C148" s="32" t="s">
         <v>48</v>
       </c>
       <c r="D148" s="7" t="s">
@@ -3435,7 +3454,7 @@
       <c r="F148" s="1"/>
     </row>
     <row r="149" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C149" s="32"/>
+      <c r="C149" s="33"/>
       <c r="D149" s="8"/>
       <c r="E149" s="8" t="s">
         <v>216</v>
@@ -3443,7 +3462,7 @@
       <c r="F149" s="1"/>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C150" s="32"/>
+      <c r="C150" s="33"/>
       <c r="D150" s="8"/>
       <c r="E150" s="9" t="s">
         <v>217</v>
@@ -3451,7 +3470,7 @@
       <c r="F150" s="1"/>
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C151" s="32"/>
+      <c r="C151" s="33"/>
       <c r="D151" s="8"/>
       <c r="E151" s="9" t="s">
         <v>218</v>
@@ -3459,7 +3478,7 @@
       <c r="F151" s="1"/>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C152" s="32"/>
+      <c r="C152" s="33"/>
       <c r="D152" s="8"/>
       <c r="E152" s="9" t="s">
         <v>219</v>
@@ -3467,7 +3486,7 @@
       <c r="F152" s="1"/>
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C153" s="32"/>
+      <c r="C153" s="33"/>
       <c r="D153" s="8"/>
       <c r="E153" s="9" t="s">
         <v>220</v>
@@ -3475,7 +3494,7 @@
       <c r="F153" s="1"/>
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C154" s="32"/>
+      <c r="C154" s="33"/>
       <c r="D154" s="8"/>
       <c r="E154" s="9" t="s">
         <v>221</v>
@@ -3483,7 +3502,7 @@
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C155" s="32"/>
+      <c r="C155" s="33"/>
       <c r="D155" s="8"/>
       <c r="E155" s="9" t="s">
         <v>97</v>
@@ -3491,7 +3510,7 @@
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C156" s="32"/>
+      <c r="C156" s="33"/>
       <c r="D156" s="19"/>
       <c r="E156" s="9" t="s">
         <v>222</v>
@@ -3499,125 +3518,125 @@
       <c r="F156" s="1"/>
     </row>
     <row r="157" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C157" s="32"/>
+      <c r="C157" s="33"/>
       <c r="E157" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="158" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C158" s="32"/>
+      <c r="C158" s="33"/>
       <c r="D158" s="5"/>
       <c r="E158" s="9" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="159" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C159" s="32"/>
+      <c r="C159" s="33"/>
       <c r="D159" s="5"/>
       <c r="E159" s="9" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C160" s="32"/>
+      <c r="C160" s="33"/>
       <c r="D160" s="5"/>
       <c r="E160" s="9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="161" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C161" s="32"/>
+      <c r="C161" s="33"/>
       <c r="D161" s="5"/>
       <c r="E161" s="9" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="162" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C162" s="32"/>
+      <c r="C162" s="33"/>
       <c r="D162" s="5"/>
       <c r="E162" s="9" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="163" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C163" s="32"/>
+      <c r="C163" s="33"/>
       <c r="D163" s="5"/>
       <c r="E163" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="164" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C164" s="32"/>
+      <c r="C164" s="33"/>
       <c r="D164" s="5"/>
       <c r="E164" s="9" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="165" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C165" s="32"/>
+      <c r="C165" s="33"/>
       <c r="D165" s="5"/>
       <c r="E165" s="9" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="166" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C166" s="32"/>
+      <c r="C166" s="33"/>
       <c r="D166" s="5"/>
       <c r="E166" s="9" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="167" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C167" s="32"/>
+      <c r="C167" s="33"/>
       <c r="D167" s="5"/>
       <c r="E167" s="9" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="168" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C168" s="32"/>
+      <c r="C168" s="33"/>
       <c r="D168" s="5"/>
       <c r="E168" s="9" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="169" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C169" s="32"/>
+      <c r="C169" s="33"/>
       <c r="D169" s="5"/>
       <c r="E169" s="9" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="170" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C170" s="32"/>
+      <c r="C170" s="33"/>
       <c r="D170" s="5"/>
       <c r="E170" s="9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="171" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C171" s="32"/>
+      <c r="C171" s="33"/>
       <c r="D171" s="5"/>
       <c r="E171" s="9" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="172" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C172" s="32"/>
+      <c r="C172" s="33"/>
       <c r="D172" s="5"/>
       <c r="E172" s="9" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="173" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C173" s="32"/>
+      <c r="C173" s="33"/>
       <c r="D173" s="5"/>
       <c r="E173" s="9" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="174" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C174" s="33"/>
+      <c r="C174" s="34"/>
       <c r="D174" s="5"/>
       <c r="E174" s="9" t="s">
         <v>240</v>
@@ -3646,7 +3665,7 @@
       </c>
     </row>
     <row r="178" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C178" s="26" t="s">
+      <c r="C178" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D178" s="22" t="s">
@@ -3663,7 +3682,7 @@
       </c>
     </row>
     <row r="179" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C179" s="26"/>
+      <c r="C179" s="27"/>
       <c r="D179" s="12" t="s">
         <v>85</v>
       </c>
@@ -3674,7 +3693,7 @@
       <c r="G179" s="9"/>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C180" s="26"/>
+      <c r="C180" s="27"/>
       <c r="D180" s="12"/>
       <c r="E180" s="9"/>
       <c r="F180" s="9" t="s">
@@ -3683,7 +3702,7 @@
       <c r="G180" s="9"/>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C181" s="26"/>
+      <c r="C181" s="27"/>
       <c r="D181" s="12"/>
       <c r="E181" s="9"/>
       <c r="F181" s="9" t="s">
@@ -3716,7 +3735,7 @@
       <c r="F184" s="10"/>
     </row>
     <row r="185" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C185" s="26" t="s">
+      <c r="C185" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D185" s="7" t="s">
@@ -3728,7 +3747,7 @@
       <c r="F185" s="10"/>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C186" s="26"/>
+      <c r="C186" s="27"/>
       <c r="D186" s="8" t="s">
         <v>247</v>
       </c>
@@ -3736,7 +3755,7 @@
       <c r="F186" s="2"/>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C187" s="26"/>
+      <c r="C187" s="27"/>
       <c r="D187" s="8" t="s">
         <v>248</v>
       </c>
@@ -3744,7 +3763,7 @@
       <c r="F187" s="2"/>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C188" s="26"/>
+      <c r="C188" s="27"/>
       <c r="D188" s="8" t="s">
         <v>249</v>
       </c>
@@ -3752,7 +3771,7 @@
       <c r="F188" s="2"/>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C189" s="26"/>
+      <c r="C189" s="27"/>
       <c r="D189" s="8" t="s">
         <v>240</v>
       </c>
@@ -3760,7 +3779,7 @@
       <c r="F189" s="2"/>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C190" s="26"/>
+      <c r="C190" s="27"/>
       <c r="D190" s="8" t="s">
         <v>222</v>
       </c>
@@ -3768,7 +3787,7 @@
       <c r="F190" s="2"/>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C191" s="26"/>
+      <c r="C191" s="27"/>
       <c r="D191" s="8" t="s">
         <v>223</v>
       </c>
@@ -3776,7 +3795,7 @@
       <c r="F191" s="2"/>
     </row>
     <row r="192" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C192" s="26"/>
+      <c r="C192" s="27"/>
       <c r="D192" s="8" t="s">
         <v>250</v>
       </c>
@@ -3784,7 +3803,7 @@
       <c r="F192" s="2"/>
     </row>
     <row r="193" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C193" s="26"/>
+      <c r="C193" s="27"/>
       <c r="D193" s="8" t="s">
         <v>66</v>
       </c>
@@ -3792,7 +3811,7 @@
       <c r="F193" s="2"/>
     </row>
     <row r="194" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C194" s="26"/>
+      <c r="C194" s="27"/>
       <c r="D194" s="8" t="s">
         <v>251</v>
       </c>
@@ -3800,98 +3819,98 @@
       <c r="F194" s="2"/>
     </row>
     <row r="195" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C195" s="26"/>
+      <c r="C195" s="27"/>
       <c r="D195" s="8" t="s">
         <v>230</v>
       </c>
       <c r="E195" s="5"/>
     </row>
     <row r="196" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C196" s="26"/>
+      <c r="C196" s="27"/>
       <c r="D196" s="8" t="s">
         <v>252</v>
       </c>
       <c r="E196" s="5"/>
     </row>
     <row r="197" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C197" s="26"/>
+      <c r="C197" s="27"/>
       <c r="D197" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E197" s="5"/>
     </row>
     <row r="198" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C198" s="26"/>
+      <c r="C198" s="27"/>
       <c r="D198" s="8" t="s">
         <v>253</v>
       </c>
       <c r="E198" s="5"/>
     </row>
     <row r="199" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C199" s="26"/>
+      <c r="C199" s="27"/>
       <c r="D199" s="8" t="s">
         <v>254</v>
       </c>
       <c r="E199" s="5"/>
     </row>
     <row r="200" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C200" s="26"/>
+      <c r="C200" s="27"/>
       <c r="D200" s="8" t="s">
         <v>255</v>
       </c>
       <c r="E200" s="5"/>
     </row>
     <row r="201" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C201" s="26"/>
+      <c r="C201" s="27"/>
       <c r="D201" s="8" t="s">
         <v>232</v>
       </c>
       <c r="E201" s="5"/>
     </row>
     <row r="202" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C202" s="26"/>
+      <c r="C202" s="27"/>
       <c r="D202" s="8" t="s">
         <v>233</v>
       </c>
       <c r="E202" s="5"/>
     </row>
     <row r="203" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C203" s="26"/>
+      <c r="C203" s="27"/>
       <c r="D203" s="8" t="s">
         <v>256</v>
       </c>
       <c r="E203" s="5"/>
     </row>
     <row r="204" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C204" s="26"/>
+      <c r="C204" s="27"/>
       <c r="D204" s="8" t="s">
         <v>257</v>
       </c>
       <c r="E204" s="5"/>
     </row>
     <row r="205" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C205" s="26"/>
+      <c r="C205" s="27"/>
       <c r="D205" s="8" t="s">
         <v>258</v>
       </c>
       <c r="E205" s="5"/>
     </row>
     <row r="206" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C206" s="26"/>
+      <c r="C206" s="27"/>
       <c r="D206" s="8" t="s">
         <v>259</v>
       </c>
       <c r="E206" s="5"/>
     </row>
     <row r="207" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C207" s="26"/>
+      <c r="C207" s="27"/>
       <c r="D207" s="8" t="s">
         <v>260</v>
       </c>
       <c r="E207" s="5"/>
     </row>
     <row r="208" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C208" s="26"/>
+      <c r="C208" s="27"/>
       <c r="D208" s="8" t="s">
         <v>105</v>
       </c>
@@ -3912,7 +3931,7 @@
       <c r="E211" s="10"/>
     </row>
     <row r="212" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C212" s="28" t="s">
+      <c r="C212" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D212" s="7" t="s">
@@ -3921,154 +3940,154 @@
       <c r="E212" s="10"/>
     </row>
     <row r="213" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C213" s="29"/>
+      <c r="C213" s="30"/>
       <c r="D213" s="8" t="s">
         <v>216</v>
       </c>
       <c r="E213" s="2"/>
     </row>
     <row r="214" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C214" s="29"/>
+      <c r="C214" s="30"/>
       <c r="D214" s="8" t="s">
         <v>218</v>
       </c>
       <c r="E214" s="2"/>
     </row>
     <row r="215" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C215" s="29"/>
+      <c r="C215" s="30"/>
       <c r="D215" s="8" t="s">
         <v>219</v>
       </c>
       <c r="E215" s="2"/>
     </row>
     <row r="216" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C216" s="29"/>
+      <c r="C216" s="30"/>
       <c r="D216" s="8" t="s">
         <v>97</v>
       </c>
       <c r="E216" s="2"/>
     </row>
     <row r="217" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C217" s="29"/>
+      <c r="C217" s="30"/>
       <c r="D217" s="8" t="s">
         <v>222</v>
       </c>
       <c r="E217" s="2"/>
     </row>
     <row r="218" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C218" s="29"/>
+      <c r="C218" s="30"/>
       <c r="D218" s="8" t="s">
         <v>223</v>
       </c>
       <c r="E218" s="2"/>
     </row>
     <row r="219" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C219" s="29"/>
+      <c r="C219" s="30"/>
       <c r="D219" s="8" t="s">
         <v>224</v>
       </c>
       <c r="E219" s="2"/>
     </row>
     <row r="220" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C220" s="29"/>
+      <c r="C220" s="30"/>
       <c r="D220" s="8" t="s">
         <v>225</v>
       </c>
       <c r="E220" s="2"/>
     </row>
     <row r="221" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C221" s="29"/>
+      <c r="C221" s="30"/>
       <c r="D221" s="8" t="s">
         <v>226</v>
       </c>
       <c r="E221" s="2"/>
     </row>
     <row r="222" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C222" s="29"/>
+      <c r="C222" s="30"/>
       <c r="D222" s="9" t="s">
         <v>227</v>
       </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C223" s="29"/>
+      <c r="C223" s="30"/>
       <c r="D223" s="9" t="s">
         <v>262</v>
       </c>
       <c r="E223" s="1"/>
     </row>
     <row r="224" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C224" s="29"/>
+      <c r="C224" s="30"/>
       <c r="D224" s="9" t="s">
         <v>231</v>
       </c>
       <c r="E224" s="1"/>
     </row>
     <row r="225" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C225" s="29"/>
+      <c r="C225" s="30"/>
       <c r="D225" s="9" t="s">
         <v>232</v>
       </c>
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C226" s="29"/>
+      <c r="C226" s="30"/>
       <c r="D226" s="9" t="s">
         <v>234</v>
       </c>
       <c r="E226" s="1"/>
     </row>
     <row r="227" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C227" s="29"/>
+      <c r="C227" s="30"/>
       <c r="D227" s="9" t="s">
         <v>235</v>
       </c>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C228" s="29"/>
+      <c r="C228" s="30"/>
       <c r="D228" s="9" t="s">
         <v>263</v>
       </c>
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C229" s="29"/>
+      <c r="C229" s="30"/>
       <c r="D229" s="9" t="s">
         <v>264</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C230" s="29"/>
+      <c r="C230" s="30"/>
       <c r="D230" s="9" t="s">
         <v>265</v>
       </c>
       <c r="E230" s="1"/>
     </row>
     <row r="231" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C231" s="29"/>
+      <c r="C231" s="30"/>
       <c r="D231" s="9" t="s">
         <v>266</v>
       </c>
       <c r="E231" s="1"/>
     </row>
     <row r="232" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C232" s="29"/>
+      <c r="C232" s="30"/>
       <c r="D232" s="9" t="s">
         <v>237</v>
       </c>
       <c r="E232" s="1"/>
     </row>
     <row r="233" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C233" s="29"/>
+      <c r="C233" s="30"/>
       <c r="D233" s="9" t="s">
         <v>239</v>
       </c>
       <c r="E233" s="1"/>
     </row>
     <row r="234" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C234" s="30"/>
+      <c r="C234" s="31"/>
       <c r="D234" s="8" t="s">
         <v>240</v>
       </c>
@@ -4079,6 +4098,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="C50:C65"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="C33:C46"/>
     <mergeCell ref="C98:C102"/>
     <mergeCell ref="C91:C94"/>
     <mergeCell ref="C185:C208"/>
@@ -4090,12 +4115,6 @@
     <mergeCell ref="C129:C133"/>
     <mergeCell ref="C117:C125"/>
     <mergeCell ref="C106:C113"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="C50:C65"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="C33:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4274,7 +4293,7 @@
       <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -4290,7 +4309,7 @@
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="8" t="s">
         <v>270</v>
       </c>
@@ -4304,7 +4323,7 @@
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="8" t="s">
         <v>197</v>
       </c>
@@ -4318,7 +4337,7 @@
       <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="8" t="s">
         <v>188</v>
       </c>
@@ -4332,7 +4351,7 @@
       <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="8" t="s">
         <v>145</v>
       </c>
@@ -4363,7 +4382,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -4373,7 +4392,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="29"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="8" t="s">
         <v>270</v>
       </c>
@@ -4381,19 +4400,19 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="29"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="8" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="8" t="s">
         <v>145</v>
       </c>
@@ -4427,7 +4446,7 @@
       </c>
     </row>
     <row r="19" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -4450,7 +4469,7 @@
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="29"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="8" t="s">
         <v>275</v>
       </c>
@@ -4469,7 +4488,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="8" t="s">
         <v>276</v>
       </c>
@@ -4484,7 +4503,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="29"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="8" t="s">
         <v>277</v>
       </c>
@@ -4497,7 +4516,7 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="29"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="8" t="s">
         <v>284</v>
       </c>
@@ -4510,7 +4529,7 @@
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="30"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="8" t="s">
         <v>285</v>
       </c>
@@ -4537,7 +4556,7 @@
       </c>
     </row>
     <row r="28" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -4548,35 +4567,35 @@
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="29"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="29"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="29"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="29"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="30"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="5"/>
       <c r="F33" s="8" t="s">
         <v>145</v>
@@ -4606,7 +4625,7 @@
       </c>
     </row>
     <row r="37" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -4620,7 +4639,7 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="29"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="8" t="s">
         <v>294</v>
       </c>
@@ -4630,7 +4649,7 @@
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="29"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="8" t="s">
         <v>295</v>
       </c>
@@ -4638,7 +4657,7 @@
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="30"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="8" t="s">
         <v>296</v>
       </c>
@@ -4666,7 +4685,7 @@
       </c>
     </row>
     <row r="44" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E44" s="7" t="s">
@@ -4674,49 +4693,49 @@
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="29"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="8" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="29"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="29"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="29"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" s="29"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D50" s="29"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="8" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="29"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="30"/>
+      <c r="D52" s="31"/>
       <c r="E52" s="8" t="s">
         <v>302</v>
       </c>
@@ -4793,7 +4812,7 @@
       <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -4807,7 +4826,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="29"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="8" t="s">
         <v>332</v>
       </c>
@@ -4819,7 +4838,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="8" t="s">
         <v>333</v>
       </c>
@@ -4829,7 +4848,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="29"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
         <v>338</v>
@@ -4837,7 +4856,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="29"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
         <v>339</v>
@@ -4845,7 +4864,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="s">
         <v>340</v>
@@ -4853,7 +4872,7 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="29"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
         <v>343</v>
@@ -4861,7 +4880,7 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="29"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
         <v>331</v>
@@ -4869,7 +4888,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="29"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
         <v>344</v>
@@ -4877,7 +4896,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="30"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
         <v>346</v>
@@ -4907,7 +4926,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="27" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -4924,7 +4943,7 @@
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="26"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="8" t="s">
         <v>332</v>
       </c>
@@ -4939,7 +4958,7 @@
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="26"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="8" t="s">
         <v>347</v>
       </c>
@@ -4952,7 +4971,7 @@
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="26"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="8" t="s">
         <v>333</v>
       </c>
@@ -4963,7 +4982,7 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="26"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="8" t="s">
         <v>348</v>
       </c>
@@ -4974,7 +4993,7 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="26"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
         <v>356</v>
@@ -5049,7 +5068,7 @@
       <c r="B3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -5069,7 +5088,7 @@
       <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
         <v>283</v>
@@ -5079,7 +5098,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="29"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
         <v>306</v>
@@ -5089,7 +5108,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="29"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
         <v>307</v>
@@ -5099,7 +5118,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="29"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
         <v>308</v>
@@ -5109,7 +5128,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
@@ -5117,7 +5136,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="30"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
@@ -5142,7 +5161,7 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -5154,7 +5173,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
         <v>320</v>
@@ -5162,7 +5181,7 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="29"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
         <v>115</v>
@@ -5170,7 +5189,7 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="29"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
         <v>321</v>
@@ -5178,7 +5197,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
         <v>311</v>
@@ -5186,7 +5205,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="29"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
         <v>171</v>
@@ -5194,21 +5213,21 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="5"/>
       <c r="F19" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="29"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="5"/>
       <c r="F20" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="30"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="5"/>
       <c r="F21" s="8" t="s">
         <v>316</v>
@@ -5237,7 +5256,7 @@
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -5254,7 +5273,7 @@
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="29"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
         <v>294</v>
@@ -5265,7 +5284,7 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="29"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
         <v>296</v>
@@ -5276,35 +5295,35 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="29"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="29"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="29"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="29"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="5"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="30"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="5"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>

</xml_diff>

<commit_message>
Commercial BI\Export LC Register_Shipment
</commit_message>
<xml_diff>
--- a/BI report view and measure tracking.xlsx
+++ b/BI report view and measure tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC4C1C2-0922-419B-9E37-8DD35342DD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9F5F4B-3C6D-40E2-AFAA-14E9256A51ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" xr2:uid="{F003A2DB-3BC2-407F-B939-8F4975B88621}"/>
+    <workbookView xWindow="2760" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="817" xr2:uid="{F003A2DB-3BC2-407F-B939-8F4975B88621}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial BI-NTDL" sheetId="7" r:id="rId1"/>
@@ -1160,7 +1160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1188,6 +1188,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1313,7 +1319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1383,6 +1389,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1407,10 +1417,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1728,7 +1738,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A14" sqref="A14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,26 +1782,26 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="35">
+      <c r="A6" s="27">
         <v>6</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="28" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="27">
         <v>7</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="28" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="37">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="38" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1826,26 +1836,26 @@
       <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="37">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="38" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="37">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="38" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="37">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="38" t="s">
         <v>360</v>
       </c>
     </row>
@@ -1874,13 +1884,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1900,7 +1910,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1917,7 +1927,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
@@ -1930,7 +1940,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1939,7 +1949,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1948,7 +1958,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1957,7 +1967,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1966,7 +1976,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1975,7 +1985,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2047,7 +2057,7 @@
       <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -2064,7 +2074,7 @@
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="8" t="s">
         <v>56</v>
       </c>
@@ -2077,7 +2087,7 @@
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="8" t="s">
         <v>57</v>
       </c>
@@ -2090,7 +2100,7 @@
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="8" t="s">
         <v>58</v>
       </c>
@@ -2103,7 +2113,7 @@
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="8" t="s">
         <v>59</v>
       </c>
@@ -2116,7 +2126,7 @@
       <c r="A8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="8" t="s">
         <v>60</v>
       </c>
@@ -2129,7 +2139,7 @@
       <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="8" t="s">
         <v>61</v>
       </c>
@@ -2138,7 +2148,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="C10" s="28"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="8" t="s">
         <v>69</v>
       </c>
@@ -2147,7 +2157,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="C11" s="28"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="8" t="s">
         <v>71</v>
       </c>
@@ -2158,7 +2168,7 @@
       <c r="A12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="8" t="s">
         <v>70</v>
       </c>
@@ -2225,7 +2235,7 @@
       <c r="A16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -2260,7 +2270,7 @@
       <c r="A17" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -2283,7 +2293,7 @@
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -2306,7 +2316,7 @@
       <c r="A19" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="30"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -2326,7 +2336,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="30"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -2349,7 +2359,7 @@
       <c r="A21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="31"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -2401,7 +2411,7 @@
       <c r="A25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="7" t="s">
@@ -2416,7 +2426,7 @@
       <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="8" t="s">
         <v>109</v>
       </c>
@@ -2427,7 +2437,7 @@
       <c r="A27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="8" t="s">
         <v>110</v>
       </c>
@@ -2438,7 +2448,7 @@
       <c r="A28" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="30"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="8" t="s">
         <v>111</v>
       </c>
@@ -2446,7 +2456,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C29" s="31"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="8" t="s">
         <v>115</v>
       </c>
@@ -2471,7 +2481,7 @@
       <c r="F32" s="10"/>
     </row>
     <row r="33" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="7" t="s">
@@ -2481,7 +2491,7 @@
       <c r="F33" s="10"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="27"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="8" t="s">
         <v>118</v>
       </c>
@@ -2489,7 +2499,7 @@
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="27"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="8" t="s">
         <v>119</v>
       </c>
@@ -2497,7 +2507,7 @@
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="27"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="8" t="s">
         <v>120</v>
       </c>
@@ -2505,7 +2515,7 @@
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="27"/>
+      <c r="C37" s="29"/>
       <c r="D37" s="8" t="s">
         <v>121</v>
       </c>
@@ -2513,7 +2523,7 @@
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="27"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="8" t="s">
         <v>128</v>
       </c>
@@ -2521,7 +2531,7 @@
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="27"/>
+      <c r="C39" s="29"/>
       <c r="D39" s="8" t="s">
         <v>122</v>
       </c>
@@ -2529,7 +2539,7 @@
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="27"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="8" t="s">
         <v>123</v>
       </c>
@@ -2537,7 +2547,7 @@
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="27"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="8" t="s">
         <v>124</v>
       </c>
@@ -2545,7 +2555,7 @@
       <c r="F41" s="2"/>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="27"/>
+      <c r="C42" s="29"/>
       <c r="D42" s="8" t="s">
         <v>125</v>
       </c>
@@ -2553,25 +2563,25 @@
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="27"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="27"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="8" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="27"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="27"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="8" t="s">
         <v>127</v>
       </c>
@@ -2594,7 +2604,7 @@
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="27" t="s">
+      <c r="C50" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D50" s="7" t="s">
@@ -2604,7 +2614,7 @@
       <c r="F50" s="10"/>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="27"/>
+      <c r="C51" s="29"/>
       <c r="D51" s="8" t="s">
         <v>132</v>
       </c>
@@ -2612,7 +2622,7 @@
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="27"/>
+      <c r="C52" s="29"/>
       <c r="D52" s="8" t="s">
         <v>133</v>
       </c>
@@ -2620,7 +2630,7 @@
       <c r="F52" s="2"/>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="27"/>
+      <c r="C53" s="29"/>
       <c r="D53" s="8" t="s">
         <v>134</v>
       </c>
@@ -2628,7 +2638,7 @@
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C54" s="27"/>
+      <c r="C54" s="29"/>
       <c r="D54" s="8" t="s">
         <v>137</v>
       </c>
@@ -2636,7 +2646,7 @@
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C55" s="27"/>
+      <c r="C55" s="29"/>
       <c r="D55" s="8" t="s">
         <v>135</v>
       </c>
@@ -2644,7 +2654,7 @@
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="27"/>
+      <c r="C56" s="29"/>
       <c r="D56" s="8" t="s">
         <v>136</v>
       </c>
@@ -2652,7 +2662,7 @@
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="27"/>
+      <c r="C57" s="29"/>
       <c r="D57" s="8" t="s">
         <v>138</v>
       </c>
@@ -2660,7 +2670,7 @@
       <c r="F57" s="2"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="27"/>
+      <c r="C58" s="29"/>
       <c r="D58" s="8" t="s">
         <v>139</v>
       </c>
@@ -2668,7 +2678,7 @@
       <c r="F58" s="2"/>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="27"/>
+      <c r="C59" s="29"/>
       <c r="D59" s="8" t="s">
         <v>140</v>
       </c>
@@ -2676,37 +2686,37 @@
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="27"/>
+      <c r="C60" s="29"/>
       <c r="D60" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
+      <c r="C61" s="29"/>
       <c r="D61" s="8" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="27"/>
+      <c r="C62" s="29"/>
       <c r="D62" s="8" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="27"/>
+      <c r="C63" s="29"/>
       <c r="D63" s="8" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C64" s="27"/>
+      <c r="C64" s="29"/>
       <c r="D64" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C65" s="27"/>
+      <c r="C65" s="29"/>
       <c r="D65" s="8" t="s">
         <v>145</v>
       </c>
@@ -2745,7 +2755,7 @@
       </c>
     </row>
     <row r="69" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D69" s="7" t="s">
@@ -2768,7 +2778,7 @@
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C70" s="30"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="8" t="s">
         <v>149</v>
       </c>
@@ -2785,7 +2795,7 @@
       <c r="I70" s="8"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="30"/>
+      <c r="C71" s="32"/>
       <c r="D71" s="8" t="s">
         <v>160</v>
       </c>
@@ -2802,7 +2812,7 @@
       <c r="I71" s="8"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C72" s="30"/>
+      <c r="C72" s="32"/>
       <c r="D72" s="8" t="s">
         <v>161</v>
       </c>
@@ -2817,7 +2827,7 @@
       <c r="I72" s="8"/>
     </row>
     <row r="73" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C73" s="30"/>
+      <c r="C73" s="32"/>
       <c r="D73" s="8" t="s">
         <v>163</v>
       </c>
@@ -2830,7 +2840,7 @@
       <c r="I73" s="8"/>
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C74" s="31"/>
+      <c r="C74" s="33"/>
       <c r="D74" s="8" t="s">
         <v>164</v>
       </c>
@@ -2876,7 +2886,7 @@
       </c>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C78" s="27" t="s">
+      <c r="C78" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D78" s="7" t="s">
@@ -2896,7 +2906,7 @@
       </c>
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C79" s="28"/>
+      <c r="C79" s="30"/>
       <c r="D79" s="8" t="s">
         <v>161</v>
       </c>
@@ -2910,7 +2920,7 @@
       <c r="H79" s="8"/>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="28"/>
+      <c r="C80" s="30"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8" t="s">
         <v>171</v>
@@ -2920,7 +2930,7 @@
       <c r="H80" s="8"/>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C81" s="28"/>
+      <c r="C81" s="30"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
         <v>119</v>
@@ -2930,7 +2940,7 @@
       <c r="H81" s="8"/>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C82" s="28"/>
+      <c r="C82" s="30"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8" t="s">
         <v>172</v>
@@ -2940,7 +2950,7 @@
       <c r="H82" s="8"/>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C83" s="28"/>
+      <c r="C83" s="30"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8" t="s">
         <v>125</v>
@@ -2950,7 +2960,7 @@
       <c r="H83" s="8"/>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C84" s="28"/>
+      <c r="C84" s="30"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8" t="s">
         <v>173</v>
@@ -2960,7 +2970,7 @@
       <c r="H84" s="8"/>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C85" s="28"/>
+      <c r="C85" s="30"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
         <v>174</v>
@@ -2970,7 +2980,7 @@
       <c r="H85" s="8"/>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C86" s="28"/>
+      <c r="C86" s="30"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
         <v>175</v>
@@ -2980,7 +2990,7 @@
       <c r="H86" s="8"/>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C87" s="28"/>
+      <c r="C87" s="30"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8" t="s">
         <v>176</v>
@@ -3010,7 +3020,7 @@
       </c>
     </row>
     <row r="91" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C91" s="29" t="s">
+      <c r="C91" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D91" s="7" t="s">
@@ -3024,7 +3034,7 @@
       </c>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C92" s="30"/>
+      <c r="C92" s="32"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8" t="s">
         <v>179</v>
@@ -3032,7 +3042,7 @@
       <c r="F92" s="8"/>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C93" s="30"/>
+      <c r="C93" s="32"/>
       <c r="D93" s="8"/>
       <c r="E93" s="8" t="s">
         <v>180</v>
@@ -3040,7 +3050,7 @@
       <c r="F93" s="8"/>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C94" s="31"/>
+      <c r="C94" s="33"/>
       <c r="D94" s="8"/>
       <c r="E94" s="8" t="s">
         <v>69</v>
@@ -3064,7 +3074,7 @@
       <c r="F97" s="10"/>
     </row>
     <row r="98" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C98" s="29" t="s">
+      <c r="C98" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D98" s="7" t="s">
@@ -3074,7 +3084,7 @@
       <c r="F98" s="10"/>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C99" s="30"/>
+      <c r="C99" s="32"/>
       <c r="D99" s="8" t="s">
         <v>186</v>
       </c>
@@ -3082,7 +3092,7 @@
       <c r="F99" s="2"/>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C100" s="30"/>
+      <c r="C100" s="32"/>
       <c r="D100" s="8" t="s">
         <v>187</v>
       </c>
@@ -3090,7 +3100,7 @@
       <c r="F100" s="2"/>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C101" s="30"/>
+      <c r="C101" s="32"/>
       <c r="D101" s="8" t="s">
         <v>188</v>
       </c>
@@ -3098,7 +3108,7 @@
       <c r="F101" s="2"/>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C102" s="31"/>
+      <c r="C102" s="33"/>
       <c r="D102" s="8" t="s">
         <v>189</v>
       </c>
@@ -3122,7 +3132,7 @@
       </c>
     </row>
     <row r="106" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C106" s="29" t="s">
+      <c r="C106" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D106" s="7" t="s">
@@ -3133,49 +3143,49 @@
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C107" s="30"/>
+      <c r="C107" s="32"/>
       <c r="D107" s="8"/>
       <c r="E107" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C108" s="30"/>
+      <c r="C108" s="32"/>
       <c r="D108" s="8"/>
       <c r="E108" s="9" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C109" s="30"/>
+      <c r="C109" s="32"/>
       <c r="D109" s="8"/>
       <c r="E109" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C110" s="30"/>
+      <c r="C110" s="32"/>
       <c r="D110" s="8"/>
       <c r="E110" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C111" s="30"/>
+      <c r="C111" s="32"/>
       <c r="D111" s="8"/>
       <c r="E111" s="9" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C112" s="30"/>
+      <c r="C112" s="32"/>
       <c r="D112" s="8"/>
       <c r="E112" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C113" s="31"/>
+      <c r="C113" s="33"/>
       <c r="D113" s="8"/>
       <c r="E113" s="9" t="s">
         <v>187</v>
@@ -3198,7 +3208,7 @@
       </c>
     </row>
     <row r="117" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C117" s="29" t="s">
+      <c r="C117" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D117" s="7" t="s">
@@ -3209,56 +3219,56 @@
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C118" s="30"/>
+      <c r="C118" s="32"/>
       <c r="D118" s="8"/>
       <c r="E118" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C119" s="30"/>
+      <c r="C119" s="32"/>
       <c r="D119" s="8"/>
       <c r="E119" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="120" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C120" s="30"/>
+      <c r="C120" s="32"/>
       <c r="D120" s="8"/>
       <c r="E120" s="9" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C121" s="30"/>
+      <c r="C121" s="32"/>
       <c r="D121" s="8"/>
       <c r="E121" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="122" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C122" s="30"/>
+      <c r="C122" s="32"/>
       <c r="D122" s="8"/>
       <c r="E122" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="123" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C123" s="30"/>
+      <c r="C123" s="32"/>
       <c r="D123" s="8"/>
       <c r="E123" s="9" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C124" s="30"/>
+      <c r="C124" s="32"/>
       <c r="D124" s="8"/>
       <c r="E124" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C125" s="31"/>
+      <c r="C125" s="33"/>
       <c r="D125" s="8"/>
       <c r="E125" s="9" t="s">
         <v>189</v>
@@ -3281,7 +3291,7 @@
       </c>
     </row>
     <row r="129" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C129" s="29" t="s">
+      <c r="C129" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D129" s="7" t="s">
@@ -3292,28 +3302,28 @@
       </c>
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C130" s="30"/>
+      <c r="C130" s="32"/>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="30"/>
+      <c r="C131" s="32"/>
       <c r="D131" s="8"/>
       <c r="E131" s="9" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C132" s="30"/>
+      <c r="C132" s="32"/>
       <c r="D132" s="8"/>
       <c r="E132" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C133" s="31"/>
+      <c r="C133" s="33"/>
       <c r="D133" s="8"/>
       <c r="E133" s="9" t="s">
         <v>197</v>
@@ -3342,7 +3352,7 @@
       </c>
     </row>
     <row r="137" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C137" s="29" t="s">
+      <c r="C137" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D137" s="7" t="s">
@@ -3359,7 +3369,7 @@
       </c>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C138" s="30"/>
+      <c r="C138" s="32"/>
       <c r="D138" s="8" t="s">
         <v>77</v>
       </c>
@@ -3370,7 +3380,7 @@
       <c r="G138" s="9"/>
     </row>
     <row r="139" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C139" s="30"/>
+      <c r="C139" s="32"/>
       <c r="D139" s="8"/>
       <c r="E139" s="9"/>
       <c r="F139" s="9" t="s">
@@ -3379,7 +3389,7 @@
       <c r="G139" s="9"/>
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C140" s="30"/>
+      <c r="C140" s="32"/>
       <c r="D140" s="8"/>
       <c r="E140" s="9"/>
       <c r="F140" s="9" t="s">
@@ -3388,7 +3398,7 @@
       <c r="G140" s="9"/>
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C141" s="30"/>
+      <c r="C141" s="32"/>
       <c r="D141" s="8"/>
       <c r="E141" s="9"/>
       <c r="F141" s="9" t="s">
@@ -3397,7 +3407,7 @@
       <c r="G141" s="9"/>
     </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C142" s="30"/>
+      <c r="C142" s="32"/>
       <c r="D142" s="8"/>
       <c r="E142" s="9"/>
       <c r="F142" s="9" t="s">
@@ -3406,7 +3416,7 @@
       <c r="G142" s="9"/>
     </row>
     <row r="143" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C143" s="30"/>
+      <c r="C143" s="32"/>
       <c r="D143" s="8"/>
       <c r="E143" s="9"/>
       <c r="F143" s="9" t="s">
@@ -3415,7 +3425,7 @@
       <c r="G143" s="9"/>
     </row>
     <row r="144" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C144" s="31"/>
+      <c r="C144" s="33"/>
       <c r="D144" s="8"/>
       <c r="E144" s="9"/>
       <c r="F144" s="9" t="s">
@@ -3442,7 +3452,7 @@
       <c r="G147" s="10"/>
     </row>
     <row r="148" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C148" s="32" t="s">
+      <c r="C148" s="34" t="s">
         <v>48</v>
       </c>
       <c r="D148" s="7" t="s">
@@ -3454,7 +3464,7 @@
       <c r="F148" s="1"/>
     </row>
     <row r="149" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C149" s="33"/>
+      <c r="C149" s="35"/>
       <c r="D149" s="8"/>
       <c r="E149" s="8" t="s">
         <v>216</v>
@@ -3462,7 +3472,7 @@
       <c r="F149" s="1"/>
     </row>
     <row r="150" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C150" s="33"/>
+      <c r="C150" s="35"/>
       <c r="D150" s="8"/>
       <c r="E150" s="9" t="s">
         <v>217</v>
@@ -3470,7 +3480,7 @@
       <c r="F150" s="1"/>
     </row>
     <row r="151" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C151" s="33"/>
+      <c r="C151" s="35"/>
       <c r="D151" s="8"/>
       <c r="E151" s="9" t="s">
         <v>218</v>
@@ -3478,7 +3488,7 @@
       <c r="F151" s="1"/>
     </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C152" s="33"/>
+      <c r="C152" s="35"/>
       <c r="D152" s="8"/>
       <c r="E152" s="9" t="s">
         <v>219</v>
@@ -3486,7 +3496,7 @@
       <c r="F152" s="1"/>
     </row>
     <row r="153" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C153" s="33"/>
+      <c r="C153" s="35"/>
       <c r="D153" s="8"/>
       <c r="E153" s="9" t="s">
         <v>220</v>
@@ -3494,7 +3504,7 @@
       <c r="F153" s="1"/>
     </row>
     <row r="154" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C154" s="33"/>
+      <c r="C154" s="35"/>
       <c r="D154" s="8"/>
       <c r="E154" s="9" t="s">
         <v>221</v>
@@ -3502,7 +3512,7 @@
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C155" s="33"/>
+      <c r="C155" s="35"/>
       <c r="D155" s="8"/>
       <c r="E155" s="9" t="s">
         <v>97</v>
@@ -3510,7 +3520,7 @@
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C156" s="33"/>
+      <c r="C156" s="35"/>
       <c r="D156" s="19"/>
       <c r="E156" s="9" t="s">
         <v>222</v>
@@ -3518,125 +3528,125 @@
       <c r="F156" s="1"/>
     </row>
     <row r="157" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C157" s="33"/>
+      <c r="C157" s="35"/>
       <c r="E157" s="9" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="158" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C158" s="33"/>
+      <c r="C158" s="35"/>
       <c r="D158" s="5"/>
       <c r="E158" s="9" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="159" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C159" s="33"/>
+      <c r="C159" s="35"/>
       <c r="D159" s="5"/>
       <c r="E159" s="9" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C160" s="33"/>
+      <c r="C160" s="35"/>
       <c r="D160" s="5"/>
       <c r="E160" s="9" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="161" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C161" s="33"/>
+      <c r="C161" s="35"/>
       <c r="D161" s="5"/>
       <c r="E161" s="9" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="162" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C162" s="33"/>
+      <c r="C162" s="35"/>
       <c r="D162" s="5"/>
       <c r="E162" s="9" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="163" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C163" s="33"/>
+      <c r="C163" s="35"/>
       <c r="D163" s="5"/>
       <c r="E163" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="164" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C164" s="33"/>
+      <c r="C164" s="35"/>
       <c r="D164" s="5"/>
       <c r="E164" s="9" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="165" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C165" s="33"/>
+      <c r="C165" s="35"/>
       <c r="D165" s="5"/>
       <c r="E165" s="9" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="166" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C166" s="33"/>
+      <c r="C166" s="35"/>
       <c r="D166" s="5"/>
       <c r="E166" s="9" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="167" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C167" s="33"/>
+      <c r="C167" s="35"/>
       <c r="D167" s="5"/>
       <c r="E167" s="9" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="168" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C168" s="33"/>
+      <c r="C168" s="35"/>
       <c r="D168" s="5"/>
       <c r="E168" s="9" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="169" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C169" s="33"/>
+      <c r="C169" s="35"/>
       <c r="D169" s="5"/>
       <c r="E169" s="9" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="170" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C170" s="33"/>
+      <c r="C170" s="35"/>
       <c r="D170" s="5"/>
       <c r="E170" s="9" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="171" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C171" s="33"/>
+      <c r="C171" s="35"/>
       <c r="D171" s="5"/>
       <c r="E171" s="9" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="172" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C172" s="33"/>
+      <c r="C172" s="35"/>
       <c r="D172" s="5"/>
       <c r="E172" s="9" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="173" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C173" s="33"/>
+      <c r="C173" s="35"/>
       <c r="D173" s="5"/>
       <c r="E173" s="9" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="174" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C174" s="34"/>
+      <c r="C174" s="36"/>
       <c r="D174" s="5"/>
       <c r="E174" s="9" t="s">
         <v>240</v>
@@ -3665,7 +3675,7 @@
       </c>
     </row>
     <row r="178" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C178" s="27" t="s">
+      <c r="C178" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D178" s="22" t="s">
@@ -3682,7 +3692,7 @@
       </c>
     </row>
     <row r="179" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C179" s="27"/>
+      <c r="C179" s="29"/>
       <c r="D179" s="12" t="s">
         <v>85</v>
       </c>
@@ -3693,7 +3703,7 @@
       <c r="G179" s="9"/>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C180" s="27"/>
+      <c r="C180" s="29"/>
       <c r="D180" s="12"/>
       <c r="E180" s="9"/>
       <c r="F180" s="9" t="s">
@@ -3702,7 +3712,7 @@
       <c r="G180" s="9"/>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C181" s="27"/>
+      <c r="C181" s="29"/>
       <c r="D181" s="12"/>
       <c r="E181" s="9"/>
       <c r="F181" s="9" t="s">
@@ -3735,7 +3745,7 @@
       <c r="F184" s="10"/>
     </row>
     <row r="185" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C185" s="27" t="s">
+      <c r="C185" s="29" t="s">
         <v>48</v>
       </c>
       <c r="D185" s="7" t="s">
@@ -3747,7 +3757,7 @@
       <c r="F185" s="10"/>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C186" s="27"/>
+      <c r="C186" s="29"/>
       <c r="D186" s="8" t="s">
         <v>247</v>
       </c>
@@ -3755,7 +3765,7 @@
       <c r="F186" s="2"/>
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C187" s="27"/>
+      <c r="C187" s="29"/>
       <c r="D187" s="8" t="s">
         <v>248</v>
       </c>
@@ -3763,7 +3773,7 @@
       <c r="F187" s="2"/>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C188" s="27"/>
+      <c r="C188" s="29"/>
       <c r="D188" s="8" t="s">
         <v>249</v>
       </c>
@@ -3771,7 +3781,7 @@
       <c r="F188" s="2"/>
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C189" s="27"/>
+      <c r="C189" s="29"/>
       <c r="D189" s="8" t="s">
         <v>240</v>
       </c>
@@ -3779,7 +3789,7 @@
       <c r="F189" s="2"/>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C190" s="27"/>
+      <c r="C190" s="29"/>
       <c r="D190" s="8" t="s">
         <v>222</v>
       </c>
@@ -3787,7 +3797,7 @@
       <c r="F190" s="2"/>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C191" s="27"/>
+      <c r="C191" s="29"/>
       <c r="D191" s="8" t="s">
         <v>223</v>
       </c>
@@ -3795,7 +3805,7 @@
       <c r="F191" s="2"/>
     </row>
     <row r="192" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C192" s="27"/>
+      <c r="C192" s="29"/>
       <c r="D192" s="8" t="s">
         <v>250</v>
       </c>
@@ -3803,7 +3813,7 @@
       <c r="F192" s="2"/>
     </row>
     <row r="193" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C193" s="27"/>
+      <c r="C193" s="29"/>
       <c r="D193" s="8" t="s">
         <v>66</v>
       </c>
@@ -3811,7 +3821,7 @@
       <c r="F193" s="2"/>
     </row>
     <row r="194" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C194" s="27"/>
+      <c r="C194" s="29"/>
       <c r="D194" s="8" t="s">
         <v>251</v>
       </c>
@@ -3819,98 +3829,98 @@
       <c r="F194" s="2"/>
     </row>
     <row r="195" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C195" s="27"/>
+      <c r="C195" s="29"/>
       <c r="D195" s="8" t="s">
         <v>230</v>
       </c>
       <c r="E195" s="5"/>
     </row>
     <row r="196" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C196" s="27"/>
+      <c r="C196" s="29"/>
       <c r="D196" s="8" t="s">
         <v>252</v>
       </c>
       <c r="E196" s="5"/>
     </row>
     <row r="197" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C197" s="27"/>
+      <c r="C197" s="29"/>
       <c r="D197" s="8" t="s">
         <v>231</v>
       </c>
       <c r="E197" s="5"/>
     </row>
     <row r="198" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C198" s="27"/>
+      <c r="C198" s="29"/>
       <c r="D198" s="8" t="s">
         <v>253</v>
       </c>
       <c r="E198" s="5"/>
     </row>
     <row r="199" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C199" s="27"/>
+      <c r="C199" s="29"/>
       <c r="D199" s="8" t="s">
         <v>254</v>
       </c>
       <c r="E199" s="5"/>
     </row>
     <row r="200" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C200" s="27"/>
+      <c r="C200" s="29"/>
       <c r="D200" s="8" t="s">
         <v>255</v>
       </c>
       <c r="E200" s="5"/>
     </row>
     <row r="201" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C201" s="27"/>
+      <c r="C201" s="29"/>
       <c r="D201" s="8" t="s">
         <v>232</v>
       </c>
       <c r="E201" s="5"/>
     </row>
     <row r="202" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C202" s="27"/>
+      <c r="C202" s="29"/>
       <c r="D202" s="8" t="s">
         <v>233</v>
       </c>
       <c r="E202" s="5"/>
     </row>
     <row r="203" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C203" s="27"/>
+      <c r="C203" s="29"/>
       <c r="D203" s="8" t="s">
         <v>256</v>
       </c>
       <c r="E203" s="5"/>
     </row>
     <row r="204" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C204" s="27"/>
+      <c r="C204" s="29"/>
       <c r="D204" s="8" t="s">
         <v>257</v>
       </c>
       <c r="E204" s="5"/>
     </row>
     <row r="205" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C205" s="27"/>
+      <c r="C205" s="29"/>
       <c r="D205" s="8" t="s">
         <v>258</v>
       </c>
       <c r="E205" s="5"/>
     </row>
     <row r="206" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C206" s="27"/>
+      <c r="C206" s="29"/>
       <c r="D206" s="8" t="s">
         <v>259</v>
       </c>
       <c r="E206" s="5"/>
     </row>
     <row r="207" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C207" s="27"/>
+      <c r="C207" s="29"/>
       <c r="D207" s="8" t="s">
         <v>260</v>
       </c>
       <c r="E207" s="5"/>
     </row>
     <row r="208" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C208" s="27"/>
+      <c r="C208" s="29"/>
       <c r="D208" s="8" t="s">
         <v>105</v>
       </c>
@@ -3931,7 +3941,7 @@
       <c r="E211" s="10"/>
     </row>
     <row r="212" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C212" s="29" t="s">
+      <c r="C212" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D212" s="7" t="s">
@@ -3940,154 +3950,154 @@
       <c r="E212" s="10"/>
     </row>
     <row r="213" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C213" s="30"/>
+      <c r="C213" s="32"/>
       <c r="D213" s="8" t="s">
         <v>216</v>
       </c>
       <c r="E213" s="2"/>
     </row>
     <row r="214" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C214" s="30"/>
+      <c r="C214" s="32"/>
       <c r="D214" s="8" t="s">
         <v>218</v>
       </c>
       <c r="E214" s="2"/>
     </row>
     <row r="215" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C215" s="30"/>
+      <c r="C215" s="32"/>
       <c r="D215" s="8" t="s">
         <v>219</v>
       </c>
       <c r="E215" s="2"/>
     </row>
     <row r="216" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C216" s="30"/>
+      <c r="C216" s="32"/>
       <c r="D216" s="8" t="s">
         <v>97</v>
       </c>
       <c r="E216" s="2"/>
     </row>
     <row r="217" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C217" s="30"/>
+      <c r="C217" s="32"/>
       <c r="D217" s="8" t="s">
         <v>222</v>
       </c>
       <c r="E217" s="2"/>
     </row>
     <row r="218" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C218" s="30"/>
+      <c r="C218" s="32"/>
       <c r="D218" s="8" t="s">
         <v>223</v>
       </c>
       <c r="E218" s="2"/>
     </row>
     <row r="219" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C219" s="30"/>
+      <c r="C219" s="32"/>
       <c r="D219" s="8" t="s">
         <v>224</v>
       </c>
       <c r="E219" s="2"/>
     </row>
     <row r="220" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C220" s="30"/>
+      <c r="C220" s="32"/>
       <c r="D220" s="8" t="s">
         <v>225</v>
       </c>
       <c r="E220" s="2"/>
     </row>
     <row r="221" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C221" s="30"/>
+      <c r="C221" s="32"/>
       <c r="D221" s="8" t="s">
         <v>226</v>
       </c>
       <c r="E221" s="2"/>
     </row>
     <row r="222" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C222" s="30"/>
+      <c r="C222" s="32"/>
       <c r="D222" s="9" t="s">
         <v>227</v>
       </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C223" s="30"/>
+      <c r="C223" s="32"/>
       <c r="D223" s="9" t="s">
         <v>262</v>
       </c>
       <c r="E223" s="1"/>
     </row>
     <row r="224" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C224" s="30"/>
+      <c r="C224" s="32"/>
       <c r="D224" s="9" t="s">
         <v>231</v>
       </c>
       <c r="E224" s="1"/>
     </row>
     <row r="225" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C225" s="30"/>
+      <c r="C225" s="32"/>
       <c r="D225" s="9" t="s">
         <v>232</v>
       </c>
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C226" s="30"/>
+      <c r="C226" s="32"/>
       <c r="D226" s="9" t="s">
         <v>234</v>
       </c>
       <c r="E226" s="1"/>
     </row>
     <row r="227" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C227" s="30"/>
+      <c r="C227" s="32"/>
       <c r="D227" s="9" t="s">
         <v>235</v>
       </c>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C228" s="30"/>
+      <c r="C228" s="32"/>
       <c r="D228" s="9" t="s">
         <v>263</v>
       </c>
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C229" s="30"/>
+      <c r="C229" s="32"/>
       <c r="D229" s="9" t="s">
         <v>264</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C230" s="30"/>
+      <c r="C230" s="32"/>
       <c r="D230" s="9" t="s">
         <v>265</v>
       </c>
       <c r="E230" s="1"/>
     </row>
     <row r="231" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C231" s="30"/>
+      <c r="C231" s="32"/>
       <c r="D231" s="9" t="s">
         <v>266</v>
       </c>
       <c r="E231" s="1"/>
     </row>
     <row r="232" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C232" s="30"/>
+      <c r="C232" s="32"/>
       <c r="D232" s="9" t="s">
         <v>237</v>
       </c>
       <c r="E232" s="1"/>
     </row>
     <row r="233" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C233" s="30"/>
+      <c r="C233" s="32"/>
       <c r="D233" s="9" t="s">
         <v>239</v>
       </c>
       <c r="E233" s="1"/>
     </row>
     <row r="234" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C234" s="31"/>
+      <c r="C234" s="33"/>
       <c r="D234" s="8" t="s">
         <v>240</v>
       </c>
@@ -4098,12 +4108,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="C69:C74"/>
-    <mergeCell ref="C50:C65"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="C33:C46"/>
     <mergeCell ref="C98:C102"/>
     <mergeCell ref="C91:C94"/>
     <mergeCell ref="C185:C208"/>
@@ -4115,6 +4119,12 @@
     <mergeCell ref="C129:C133"/>
     <mergeCell ref="C117:C125"/>
     <mergeCell ref="C106:C113"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="C50:C65"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="C33:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4293,7 +4303,7 @@
       <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -4309,7 +4319,7 @@
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="8" t="s">
         <v>270</v>
       </c>
@@ -4323,7 +4333,7 @@
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="8" t="s">
         <v>197</v>
       </c>
@@ -4337,7 +4347,7 @@
       <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="8" t="s">
         <v>188</v>
       </c>
@@ -4351,7 +4361,7 @@
       <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="31"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="8" t="s">
         <v>145</v>
       </c>
@@ -4382,7 +4392,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="7" t="s">
@@ -4392,7 +4402,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="30"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="8" t="s">
         <v>270</v>
       </c>
@@ -4400,19 +4410,19 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="30"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="8" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="30"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="31"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="8" t="s">
         <v>145</v>
       </c>
@@ -4446,7 +4456,7 @@
       </c>
     </row>
     <row r="19" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="7" t="s">
@@ -4469,7 +4479,7 @@
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D20" s="30"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="8" t="s">
         <v>275</v>
       </c>
@@ -4488,7 +4498,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D21" s="30"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="8" t="s">
         <v>276</v>
       </c>
@@ -4503,7 +4513,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D22" s="30"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="8" t="s">
         <v>277</v>
       </c>
@@ -4516,7 +4526,7 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="30"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="8" t="s">
         <v>284</v>
       </c>
@@ -4529,7 +4539,7 @@
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D24" s="31"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="8" t="s">
         <v>285</v>
       </c>
@@ -4556,7 +4566,7 @@
       </c>
     </row>
     <row r="28" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -4567,35 +4577,35 @@
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="30"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="30"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="30"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D32" s="30"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="31"/>
+      <c r="D33" s="33"/>
       <c r="E33" s="5"/>
       <c r="F33" s="8" t="s">
         <v>145</v>
@@ -4625,7 +4635,7 @@
       </c>
     </row>
     <row r="37" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -4639,7 +4649,7 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="30"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="8" t="s">
         <v>294</v>
       </c>
@@ -4649,7 +4659,7 @@
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D39" s="30"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="8" t="s">
         <v>295</v>
       </c>
@@ -4657,7 +4667,7 @@
       <c r="G39" s="9"/>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="31"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="8" t="s">
         <v>296</v>
       </c>
@@ -4685,7 +4695,7 @@
       </c>
     </row>
     <row r="44" spans="4:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E44" s="7" t="s">
@@ -4693,49 +4703,49 @@
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="30"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="8" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="30"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="30"/>
+      <c r="D47" s="32"/>
       <c r="E47" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="30"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D49" s="30"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D50" s="30"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="8" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="30"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="31"/>
+      <c r="D52" s="33"/>
       <c r="E52" s="8" t="s">
         <v>302</v>
       </c>
@@ -4812,7 +4822,7 @@
       <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -4826,7 +4836,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="30"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="8" t="s">
         <v>332</v>
       </c>
@@ -4838,7 +4848,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D5" s="30"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="8" t="s">
         <v>333</v>
       </c>
@@ -4848,7 +4858,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="30"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
         <v>338</v>
@@ -4856,7 +4866,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D7" s="30"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
         <v>339</v>
@@ -4864,7 +4874,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="30"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="s">
         <v>340</v>
@@ -4872,7 +4882,7 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="30"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
         <v>343</v>
@@ -4880,7 +4890,7 @@
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="30"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
         <v>331</v>
@@ -4888,7 +4898,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D11" s="30"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
         <v>344</v>
@@ -4896,7 +4906,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="31"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
         <v>346</v>
@@ -4926,7 +4936,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="29" t="s">
         <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -4943,7 +4953,7 @@
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="27"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="8" t="s">
         <v>332</v>
       </c>
@@ -4958,7 +4968,7 @@
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="27"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="8" t="s">
         <v>347</v>
       </c>
@@ -4971,7 +4981,7 @@
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="27"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="8" t="s">
         <v>333</v>
       </c>
@@ -4982,7 +4992,7 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="27"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="8" t="s">
         <v>348</v>
       </c>
@@ -4993,7 +5003,7 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="27"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
         <v>356</v>
@@ -5068,7 +5078,7 @@
       <c r="B3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -5088,7 +5098,7 @@
       <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
         <v>283</v>
@@ -5098,7 +5108,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="30"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
         <v>306</v>
@@ -5108,7 +5118,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="30"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
         <v>307</v>
@@ -5118,7 +5128,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="30"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
         <v>308</v>
@@ -5128,7 +5138,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="30"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
@@ -5136,7 +5146,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="31"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
@@ -5161,7 +5171,7 @@
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -5173,7 +5183,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="30"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
         <v>320</v>
@@ -5181,7 +5191,7 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="30"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
         <v>115</v>
@@ -5189,7 +5199,7 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="30"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
         <v>321</v>
@@ -5197,7 +5207,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="30"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
         <v>311</v>
@@ -5205,7 +5215,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="30"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
         <v>171</v>
@@ -5213,21 +5223,21 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="30"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="5"/>
       <c r="F19" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" s="30"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="5"/>
       <c r="F20" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="31"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="5"/>
       <c r="F21" s="8" t="s">
         <v>316</v>
@@ -5256,7 +5266,7 @@
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="31" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="7" t="s">
@@ -5273,7 +5283,7 @@
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="30"/>
+      <c r="D26" s="32"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
         <v>294</v>
@@ -5284,7 +5294,7 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="30"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
         <v>296</v>
@@ -5295,35 +5305,35 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D28" s="30"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D29" s="30"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D30" s="30"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D31" s="30"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="5"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="31"/>
+      <c r="D32" s="33"/>
       <c r="E32" s="5"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>

</xml_diff>